<commit_message>
Fix báo cáo excel
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/PXK.xlsx
+++ b/src/main/resources/report_templates/PXK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA5C4B-69D4-4EF5-AEFE-2C2933948B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC093DB-CCA4-4A91-B35D-C0AC0C47E517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="576" windowWidth="23256" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -756,34 +756,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -820,11 +805,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,8 +1140,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1168,11 +1168,11 @@
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1185,11 +1185,11 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1198,21 +1198,21 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
     </row>
     <row r="4" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
     </row>
     <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
@@ -1223,32 +1223,32 @@
       <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1313,40 +1313,40 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="60" t="s">
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="48" t="s">
+      <c r="J15" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="57" t="s">
+      <c r="K15" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="58"/>
+      <c r="L15" s="53"/>
     </row>
     <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="56"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="51"/>
       <c r="K16" s="44" t="s">
         <v>13</v>
       </c>
@@ -1358,15 +1358,15 @@
       <c r="A17" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="64"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="59"/>
       <c r="I17" s="40" t="s">
         <v>41</v>
       </c>
@@ -1382,13 +1382,13 @@
     </row>
     <row r="18" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="67"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="62"/>
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
       <c r="K18" s="42"/>
@@ -1478,53 +1478,53 @@
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J25" s="54" t="s">
+      <c r="J25" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
     </row>
     <row r="26" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68" t="s">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68" t="s">
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="68"/>
+      <c r="L26" s="46"/>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
     </row>
     <row r="27" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69" t="s">
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69" t="s">
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="69"/>
+      <c r="L27" s="47"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
@@ -1546,20 +1546,20 @@
       <c r="O28" s="27"/>
     </row>
     <row r="29" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68" t="s">
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="L29" s="68"/>
+      <c r="L29" s="46"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
@@ -1582,6 +1582,20 @@
     <row r="64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="B15:H16"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
@@ -1597,20 +1611,6 @@
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="B15:H16"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.20833333333333334" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>